<commit_message>
Commit folders to store PDF files downloaded
</commit_message>
<xml_diff>
--- a/configs/files/publication_params_training.xlsx
+++ b/configs/files/publication_params_training.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/ai-development/genetics-usecase/prompt-automation/configs/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/ai-genetics-functional-paper/configs/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BC7C1-20A7-1B4F-A7DE-8AF64648E947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D59B43-6B17-B540-B183-1073A1A91AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,9 +481,6 @@
     <t>variant_aliases</t>
   </si>
   <si>
-    <t>PDF-files/test_set</t>
-  </si>
-  <si>
     <t>expected_outcomes</t>
   </si>
   <si>
@@ -1016,6 +1013,9 @@
   </si>
   <si>
     <t>Functional effects oftaugene mutationsDN296and N296H.pdf</t>
+  </si>
+  <si>
+    <t>PDF-files/training_set</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1364,12 +1364,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1533,23 +1527,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1910,1077 +1899,1081 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="159.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="49.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="29" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G3" s="4" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="F24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="F27" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F30" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="G30" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
-        <v>168</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>169</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>170</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>171</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>175</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
-        <v>177</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>178</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" t="s">
-        <v>179</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F35" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F24" t="s">
-        <v>180</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F25" t="s">
-        <v>180</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" t="s">
-        <v>180</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" t="s">
-        <v>180</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" t="s">
-        <v>181</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" t="s">
-        <v>168</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>153</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" t="s">
-        <v>183</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>153</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>184</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" t="s">
-        <v>185</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" t="s">
-        <v>153</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" t="s">
-        <v>186</v>
-      </c>
-      <c r="G35" s="4" t="s">
+      <c r="F37" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" t="s">
-        <v>187</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" t="s">
-        <v>153</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="G38" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" t="s">
-        <v>189</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" t="s">
-        <v>189</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" t="s">
-        <v>153</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="G42" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="G43" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G44" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="G45" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" t="s">
-        <v>194</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F47" s="1"/>
+      <c r="F47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Simplify names of classifications in configuration files
</commit_message>
<xml_diff>
--- a/configs/files/publication_params_training.xlsx
+++ b/configs/files/publication_params_training.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/ai-genetics-functional-paper/configs/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiyeonshin/Documents/AI-Projects/branch/ai-genetics-functional-paper/configs/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D59B43-6B17-B540-B183-1073A1A91AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B23D20-5A5D-FC46-9773-5814813856AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="195">
   <si>
     <t>id</t>
   </si>
@@ -484,24 +484,6 @@
     <t>expected_outcomes</t>
   </si>
   <si>
-    <t>Assays Indicate Variant Is Pathogenic</t>
-  </si>
-  <si>
-    <t>Assays indicate Variant has Intermediate Function.</t>
-  </si>
-  <si>
-    <t>Assays Indicate Variant is Benign.</t>
-  </si>
-  <si>
-    <t>Assays are inconclusive.</t>
-  </si>
-  <si>
-    <t>Assays Indicate Variant has Intermediate Function</t>
-  </si>
-  <si>
-    <t>Assay information not present.</t>
-  </si>
-  <si>
     <r>
       <t>1A</t>
     </r>
@@ -1016,13 +998,28 @@
   </si>
   <si>
     <t>PDF-files/training_set</t>
+  </si>
+  <si>
+    <t>Pathogenic</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Benign</t>
+  </si>
+  <si>
+    <t>No Assays</t>
+  </si>
+  <si>
+    <t>Inconclusive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1175,14 +1172,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1527,20 +1516,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1600,9 +1585,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1640,7 +1625,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1746,7 +1731,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1888,7 +1873,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1898,1082 +1883,1079 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="29" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.5" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
         <v>160</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G11" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="F24" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F26" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="F27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="F28" t="s">
+        <v>173</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="F30" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="F35" t="s">
+        <v>179</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="F36" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="F37" t="s">
         <v>181</v>
       </c>
-      <c r="G31" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="G37" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" t="s">
         <v>182</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="G38" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" t="s">
         <v>183</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="G42" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
         <v>184</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="G43" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
         <v>185</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="G44" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F45" t="s">
         <v>186</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="G45" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" t="s">
         <v>187</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F47" s="2"/>
+      <c r="F47" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>